<commit_message>
Incorporated modified MCGLT and BVTStL files for federal analysis
</commit_message>
<xml_diff>
--- a/InputData/trans/BVTStL/Boolean Veh Types Subject to LCFS.xlsx
+++ b/InputData/trans/BVTStL/Boolean Veh Types Subject to LCFS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipL\InputData\trans\BVTStL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\US Modeling Projects\eps-2.0.0-us - Warren\InputData\trans\BVTStL\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -554,7 +554,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,10 +602,10 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -613,10 +613,10 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -624,10 +624,10 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated trans/BVTStL so that all vehicle types except aircraft are subject to the LCFS
</commit_message>
<xml_diff>
--- a/InputData/trans/BVTStL/Boolean Veh Types Subject to LCFS.xlsx
+++ b/InputData/trans/BVTStL/Boolean Veh Types Subject to LCFS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipL\InputData\trans\BVTStL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-us\InputData\trans\BVTStL\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Source:</t>
   </si>
@@ -76,25 +76,13 @@
     <t>Page 15</t>
   </si>
   <si>
-    <t>Based on the California LCFS, we choose to exempt aircraft,</t>
-  </si>
-  <si>
-    <t>rail, and ship modes.  All three on-road modes (LDVs, HDVs,</t>
-  </si>
-  <si>
-    <t>motorbikes) are considered to be subject to the LCFS.</t>
-  </si>
-  <si>
-    <t>(California appears to include some ships and rail under</t>
-  </si>
-  <si>
-    <t>their LCFS, but we do not do so here.)</t>
-  </si>
-  <si>
     <t>BVTStL Boolean Vehicle Types Subject to LCFS</t>
   </si>
   <si>
     <t>(Boolean)</t>
+  </si>
+  <si>
+    <t>Based on the California LCFS, we choose to exempt aircraft.</t>
   </si>
 </sst>
 </file>
@@ -451,18 +439,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -470,74 +460,54 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B4" s="2">
         <v>2015</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -554,19 +524,19 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.1328125" customWidth="1"/>
+    <col min="2" max="2" width="15.1328125" customWidth="1"/>
+    <col min="3" max="3" width="13.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>8</v>
@@ -575,7 +545,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -586,7 +556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -597,7 +567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -608,29 +578,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
Remove aviation exemption from LCFS
</commit_message>
<xml_diff>
--- a/InputData/trans/BVTStL/Boolean Veh Types Subject to LCFS.xlsx
+++ b/InputData/trans/BVTStL/Boolean Veh Types Subject to LCFS.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-us\InputData\trans\BVTStL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\trans\BVTStL\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C69D041D-616D-4752-98E5-B1099603DCB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="23955" windowHeight="11325"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Source:</t>
   </si>
@@ -64,31 +65,19 @@
     <t>types will be unaffected by the LCFS.</t>
   </si>
   <si>
-    <t>California Air Resources Board</t>
-  </si>
-  <si>
-    <t>Low Carbon Fuel Standard: Final Regulation Order</t>
-  </si>
-  <si>
-    <t>https://www.arb.ca.gov/regact/2015/lcfs2015/lcfsfinalregorder.pdf</t>
-  </si>
-  <si>
-    <t>Page 15</t>
-  </si>
-  <si>
     <t>BVTStL Boolean Vehicle Types Subject to LCFS</t>
   </si>
   <si>
     <t>(Boolean)</t>
   </si>
   <si>
-    <t>Based on the California LCFS, we choose to exempt aircraft.</t>
+    <t>None</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -126,12 +115,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -228,6 +214,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -263,6 +266,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -438,76 +458,51 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="A4" sqref="A4:XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B4" s="2">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A9" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -517,35 +512,35 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.1328125" customWidth="1"/>
-    <col min="2" max="2" width="15.1328125" customWidth="1"/>
-    <col min="3" max="3" width="13.1328125" customWidth="1"/>
+    <col min="1" max="1" width="14.08984375" customWidth="1"/>
+    <col min="2" max="2" width="15.08984375" customWidth="1"/>
+    <col min="3" max="3" width="13.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -556,7 +551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -567,18 +562,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -589,7 +584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -600,7 +595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
Revert "Remove aviation exemption from LCFS"
This reverts commit 02f388e7575ec55005a59bf245fdac700fbbcb1b.
</commit_message>
<xml_diff>
--- a/InputData/trans/BVTStL/Boolean Veh Types Subject to LCFS.xlsx
+++ b/InputData/trans/BVTStL/Boolean Veh Types Subject to LCFS.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\trans\BVTStL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-us\InputData\trans\BVTStL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C69D041D-616D-4752-98E5-B1099603DCB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="23955" windowHeight="11325"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Source:</t>
   </si>
@@ -65,19 +64,31 @@
     <t>types will be unaffected by the LCFS.</t>
   </si>
   <si>
+    <t>California Air Resources Board</t>
+  </si>
+  <si>
+    <t>Low Carbon Fuel Standard: Final Regulation Order</t>
+  </si>
+  <si>
+    <t>https://www.arb.ca.gov/regact/2015/lcfs2015/lcfsfinalregorder.pdf</t>
+  </si>
+  <si>
+    <t>Page 15</t>
+  </si>
+  <si>
     <t>BVTStL Boolean Vehicle Types Subject to LCFS</t>
   </si>
   <si>
     <t>(Boolean)</t>
   </si>
   <si>
-    <t>None</t>
+    <t>Based on the California LCFS, we choose to exempt aircraft.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -115,9 +126,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -214,23 +228,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -266,23 +263,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -458,51 +438,76 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD7"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B4" s="2">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A9" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -512,35 +517,35 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14.08984375" customWidth="1"/>
-    <col min="2" max="2" width="15.08984375" customWidth="1"/>
-    <col min="3" max="3" width="13.08984375" customWidth="1"/>
+    <col min="1" max="1" width="14.1328125" customWidth="1"/>
+    <col min="2" max="2" width="15.1328125" customWidth="1"/>
+    <col min="3" max="3" width="13.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -551,7 +556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -562,18 +567,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -584,7 +589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -595,7 +600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>7</v>
       </c>

</xml_diff>